<commit_message>
add draft interactive binning page UI
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D20FCE-E2DD-41AA-AA3C-F71E3845A1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D009652-CC56-4BF1-91FB-D3B8B4FB6145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>Display only predictor variable confirmed in 'Confirm Inpute Dataset' page in the dropdown</t>
+  </si>
+  <si>
+    <t>Show a dropdown for selecting an automated binning algorithm</t>
+  </si>
+  <si>
+    <t>Update the description of the automated binning algorithm selected based on dropdown value</t>
+  </si>
+  <si>
+    <t>Show mixed chart</t>
+  </si>
+  <si>
+    <t>Show control panel</t>
+  </si>
+  <si>
+    <t>Show initial (after) summary statistics table panel</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -496,14 +514,14 @@
   <dimension ref="A1:AA44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.08984375" style="5" bestFit="1" customWidth="1"/>
@@ -1092,13 +1110,109 @@
       <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="5">
+        <v>44978</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="5">
+        <v>44978</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="32" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add preview page sections layout
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D009652-CC56-4BF1-91FB-D3B8B4FB6145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E24397-A07A-4173-9FE8-F3255BDAD206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -147,10 +147,22 @@
     <t>Show control panel</t>
   </si>
   <si>
-    <t>Show initial (after) summary statistics table panel</t>
-  </si>
-  <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Preview &amp; Download Settings</t>
+  </si>
+  <si>
+    <t>Show preview dataset</t>
+  </si>
+  <si>
+    <t>Download json bin settings button</t>
+  </si>
+  <si>
+    <t>(Backend)</t>
+  </si>
+  <si>
+    <t>Initial binning &amp; save result to shared storage - treat every value as a unique bin</t>
   </si>
 </sst>
 </file>
@@ -513,14 +525,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
@@ -1163,7 +1175,7 @@
         <v>9</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1180,7 +1192,7 @@
         <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1188,13 +1200,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="5">
+        <v>44980</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1202,7 +1220,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="5">
+        <v>44980</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1210,7 +1240,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="5">
+        <v>44980</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
show boundary error message
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B615FC38-E25C-4971-9B72-22EDC5A5CE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3352354-D62C-4786-AC46-1FDB7E0A777B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,8 +744,8 @@
     <col min="3" max="3" width="82.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="94.6328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1057,6 +1057,15 @@
       <c r="C13" t="s">
         <v>91</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5">
+        <v>45004</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
@@ -1068,6 +1077,15 @@
       <c r="C14" t="s">
         <v>81</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="5">
+        <v>45004</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
@@ -1368,6 +1386,15 @@
       </c>
       <c r="C28" t="s">
         <v>89</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="5">
+        <v>45004</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
validate categorical overlapping def
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3352354-D62C-4786-AC46-1FDB7E0A777B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A01593-B80D-4009-9CA4-B092D585D337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -300,10 +300,19 @@
     <t>If upper bound &gt; lower bound is violated, show error message</t>
   </si>
   <si>
-    <t>Validate any overlapping user input between bad &amp; indeterminate before data is saved</t>
-  </si>
-  <si>
     <t>Validate if any column with dtype 'object' marked as numerical before save</t>
+  </si>
+  <si>
+    <t>Validate any overlapping numerical user input between bad &amp; indeterminate before data is saved</t>
+  </si>
+  <si>
+    <t>Validate any overlapping categorical user input between bad &amp; indeterminate before data is saved</t>
+  </si>
+  <si>
+    <t>Show error message when overlapping numerical user input</t>
+  </si>
+  <si>
+    <t>Show error message when overlapping categorical user input</t>
   </si>
 </sst>
 </file>
@@ -734,14 +743,14 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
@@ -1055,7 +1064,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1405,7 +1414,7 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1416,7 +1425,16 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>92</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="5">
+        <v>45004</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1427,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1438,7 +1456,16 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>94</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="5">
+        <v>45004</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1449,17 +1476,29 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
+      <c r="B34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
validate numerical overlapping def
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A01593-B80D-4009-9CA4-B092D585D337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10867E7D-91C5-4563-9005-1774C2149025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,6 +1416,15 @@
       <c r="C29" t="s">
         <v>91</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="5">
+        <v>45004</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
@@ -1446,6 +1455,15 @@
       </c>
       <c r="C31" t="s">
         <v>93</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="5">
+        <v>45004</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
setup binning structure, preview df, good bad stat
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10867E7D-91C5-4563-9005-1774C2149025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B09A125-91E6-4E3A-8882-25210E917DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -313,6 +313,39 @@
   </si>
   <si>
     <t>Show error message when overlapping categorical user input</t>
+  </si>
+  <si>
+    <t>(Automated Binning)</t>
+  </si>
+  <si>
+    <t>Show preview dataset based on binned_df in storage</t>
+  </si>
+  <si>
+    <t>Perform no binning</t>
+  </si>
+  <si>
+    <t>Compute sample indeterminate count</t>
+  </si>
+  <si>
+    <t>Compute sample good count, population good count, and population bad count</t>
+  </si>
+  <si>
+    <t>Compute sample bad count</t>
+  </si>
+  <si>
+    <t>Perform equal-width binning with width</t>
+  </si>
+  <si>
+    <t>Perform equal-width binning with number of bins</t>
+  </si>
+  <si>
+    <t>Perform equal-frequency binning with frequency</t>
+  </si>
+  <si>
+    <t>Perform equal-frequency binning with number of bins</t>
+  </si>
+  <si>
+    <t>Perform binning with bins settings</t>
   </si>
 </sst>
 </file>
@@ -740,22 +773,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA39"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" style="3" customWidth="1"/>
     <col min="3" max="3" width="86.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="94.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="106.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1101,10 +1134,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -1113,7 +1146,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="5">
-        <v>45003</v>
+        <v>45004</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>8</v>
@@ -1127,7 +1160,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1136,7 +1169,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="5">
-        <v>45001</v>
+        <v>45003</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>8</v>
@@ -1150,7 +1183,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
@@ -1159,7 +1192,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="5">
-        <v>45003</v>
+        <v>45001</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>8</v>
@@ -1173,13 +1206,19 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>66</v>
+        <v>12</v>
+      </c>
+      <c r="F18" s="5">
+        <v>45003</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1190,19 +1229,13 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="5">
-        <v>45003</v>
+        <v>66</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1213,7 +1246,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
@@ -1236,7 +1269,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -1245,7 +1278,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="5">
-        <v>45001</v>
+        <v>45003</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>8</v>
@@ -1259,7 +1292,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>8</v>
@@ -1282,16 +1315,19 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>66</v>
+        <v>12</v>
+      </c>
+      <c r="F23" s="5">
+        <v>45001</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1302,19 +1338,16 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="5">
-        <v>45003</v>
+        <v>66</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1325,7 +1358,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>8</v>
@@ -1348,7 +1381,7 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>8</v>
@@ -1371,7 +1404,7 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
@@ -1380,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="5">
-        <v>45004</v>
+        <v>45003</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>8</v>
@@ -1394,7 +1427,7 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
@@ -1404,6 +1437,9 @@
       </c>
       <c r="F28" s="5">
         <v>45004</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1414,7 +1450,7 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
@@ -1434,7 +1470,7 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
@@ -1454,7 +1490,7 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
@@ -1474,7 +1510,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
@@ -1486,7 +1522,7 @@
         <v>45004</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1494,10 +1530,19 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="5">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1507,8 +1552,17 @@
       <c r="C34" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="5">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1518,25 +1572,197 @@
       <c r="C35" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="5">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="5">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="5">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compute good bad count
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B09A125-91E6-4E3A-8882-25210E917DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE2148A-D289-4349-BC08-B9B76ED27851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,28 @@
     <sheet name="Appendix (research)" sheetId="2" r:id="rId3"/>
     <sheet name="Old Backlog" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -775,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1592,6 +1603,15 @@
       <c r="C36" t="s">
         <v>100</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="5">
+        <v>45005</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
@@ -1603,6 +1623,15 @@
       <c r="C37" t="s">
         <v>98</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="5">
+        <v>45005</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
@@ -1613,6 +1642,15 @@
       </c>
       <c r="C38" t="s">
         <v>99</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="5">
+        <v>45005</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add/remove/save/validate defs, show error
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE2148A-D289-4349-BC08-B9B76ED27851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773AB044-3E93-4DBF-9FEB-3C9687AA2CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -266,9 +266,6 @@
     <t>Show only categorical variable in dataset as dropdown options for bad categorical variables</t>
   </si>
   <si>
-    <t>Require installation of dash-renderer in code environment, not sure why but even in local computer, intallation gets error</t>
-  </si>
-  <si>
     <t>Update categorical options based on dropdown value</t>
   </si>
   <si>
@@ -357,6 +354,18 @@
   </si>
   <si>
     <t>Perform binning with bins settings</t>
+  </si>
+  <si>
+    <t>18/3/2023 (Amend: 21/3/2023)</t>
+  </si>
+  <si>
+    <t>19/3/2023 (Amend: 21/3/2023)</t>
+  </si>
+  <si>
+    <t>20/3/2023 (Amend: 21/3/2023)</t>
+  </si>
+  <si>
+    <t>Validate weights to be numeric &amp; non-negative, show error message if not</t>
   </si>
 </sst>
 </file>
@@ -786,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,7 +806,7 @@
     <col min="3" max="3" width="86.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="106.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -1108,7 +1117,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1128,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1148,7 +1157,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -1171,7 +1180,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1217,7 +1226,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
@@ -1240,13 +1249,16 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>75</v>
+        <v>12</v>
+      </c>
+      <c r="F19" s="5">
+        <v>45006</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1257,7 +1269,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
@@ -1265,8 +1277,8 @@
       <c r="E20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="5">
-        <v>45003</v>
+      <c r="F20" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>8</v>
@@ -1280,7 +1292,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -1288,8 +1300,8 @@
       <c r="E21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="5">
-        <v>45003</v>
+      <c r="F21" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>8</v>
@@ -1349,16 +1361,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1369,7 +1375,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>8</v>
@@ -1392,7 +1398,7 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>8</v>
@@ -1400,8 +1406,8 @@
       <c r="E26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="5">
-        <v>45003</v>
+      <c r="F26" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>8</v>
@@ -1415,7 +1421,7 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
@@ -1438,7 +1444,7 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
@@ -1446,8 +1452,8 @@
       <c r="E28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="5">
-        <v>45004</v>
+      <c r="F28" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>8</v>
@@ -1461,7 +1467,7 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
@@ -1469,8 +1475,8 @@
       <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="5">
-        <v>45004</v>
+      <c r="F29" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1481,7 +1487,7 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
@@ -1489,8 +1495,8 @@
       <c r="E30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="5">
-        <v>45004</v>
+      <c r="F30" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1501,7 +1507,7 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
@@ -1509,8 +1515,8 @@
       <c r="E31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="5">
-        <v>45004</v>
+      <c r="F31" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1521,7 +1527,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
@@ -1529,8 +1535,8 @@
       <c r="E32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="5">
-        <v>45004</v>
+      <c r="F32" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1541,7 +1547,7 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
@@ -1549,8 +1555,8 @@
       <c r="E33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="5">
-        <v>45004</v>
+      <c r="F33" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1561,7 +1567,7 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
@@ -1601,7 +1607,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
@@ -1621,7 +1627,7 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>8</v>
@@ -1641,7 +1647,7 @@
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
@@ -1649,8 +1655,8 @@
       <c r="E38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="5">
-        <v>45005</v>
+      <c r="F38" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1658,10 +1664,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
@@ -1678,10 +1684,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1689,10 +1695,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1700,10 +1706,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1711,10 +1717,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1722,16 +1728,31 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
+      <c r="B45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="5">
+        <v>45006</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
@@ -1741,7 +1762,7 @@
         <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add select var to bin, and auto bin panel UI
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773AB044-3E93-4DBF-9FEB-3C9687AA2CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A79D01-2637-4AEC-8C43-9A6ED5C27B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -366,6 +366,24 @@
   </si>
   <si>
     <t>Validate weights to be numeric &amp; non-negative, show error message if not</t>
+  </si>
+  <si>
+    <t>Show select binning variable dropdown</t>
+  </si>
+  <si>
+    <t>Show select automated binning algorithm panel</t>
+  </si>
+  <si>
+    <t>Include only columns chosen by user in confirm input dataset page in the binning var dropdown</t>
+  </si>
+  <si>
+    <t>Change the layout based on automated binning algorithm selected by user</t>
+  </si>
+  <si>
+    <t>Press refresh button in automated binning panel to trigger binning &amp; save temp binned df to storage</t>
+  </si>
+  <si>
+    <t>Press refresh button in automated binning panel to save temp bins_settings to storage</t>
   </si>
 </sst>
 </file>
@@ -795,15 +813,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="86.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.453125" style="5" bestFit="1" customWidth="1"/>
@@ -1363,8 +1381,14 @@
       <c r="C24" t="s">
         <v>75</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E24" s="3" t="s">
-        <v>70</v>
+        <v>12</v>
+      </c>
+      <c r="F24" s="5">
+        <v>45006</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1664,10 +1688,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
@@ -1676,7 +1700,7 @@
         <v>12</v>
       </c>
       <c r="F39" s="5">
-        <v>45004</v>
+        <v>45006</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1684,10 +1708,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="5">
+        <v>45004</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1695,10 +1728,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>109</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="5">
+        <v>45006</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1706,10 +1748,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>110</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="5">
+        <v>45006</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1717,10 +1768,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>111</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="5">
+        <v>45006</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1728,10 +1788,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>112</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="5">
+        <v>45006</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1739,19 +1808,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="5">
-        <v>45006</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1759,67 +1819,103 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="5">
-        <v>45004</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
+      <c r="B47" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="5">
+        <v>45004</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B49" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B51" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
update auto bin panel UI
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A79D01-2637-4AEC-8C43-9A6ED5C27B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FDB845-A827-41DE-8DBE-03E47E0C9071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
plan for interactive binning
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FDB845-A827-41DE-8DBE-03E47E0C9071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB93194-FCED-416F-8E82-EF5CE1517E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -378,12 +378,6 @@
   </si>
   <si>
     <t>Change the layout based on automated binning algorithm selected by user</t>
-  </si>
-  <si>
-    <t>Press refresh button in automated binning panel to trigger binning &amp; save temp binned df to storage</t>
-  </si>
-  <si>
-    <t>Press refresh button in automated binning panel to save temp bins_settings to storage</t>
   </si>
 </sst>
 </file>
@@ -814,7 +808,7 @@
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1807,78 +1801,33 @@
       <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="5">
-        <v>45004</v>
-      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -1886,10 +1835,19 @@
         <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="5">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -1897,27 +1855,51 @@
         <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement equal width/freq, add design
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB93194-FCED-416F-8E82-EF5CE1517E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A120448C-1079-40BD-8AAB-D3CEB22ADD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -341,21 +341,6 @@
     <t>Compute sample bad count</t>
   </si>
   <si>
-    <t>Perform equal-width binning with width</t>
-  </si>
-  <si>
-    <t>Perform equal-width binning with number of bins</t>
-  </si>
-  <si>
-    <t>Perform equal-frequency binning with frequency</t>
-  </si>
-  <si>
-    <t>Perform equal-frequency binning with number of bins</t>
-  </si>
-  <si>
-    <t>Perform binning with bins settings</t>
-  </si>
-  <si>
     <t>18/3/2023 (Amend: 21/3/2023)</t>
   </si>
   <si>
@@ -378,13 +363,76 @@
   </si>
   <si>
     <t>Change the layout based on automated binning algorithm selected by user</t>
+  </si>
+  <si>
+    <t>Perform equal-width binning with width (numerical)</t>
+  </si>
+  <si>
+    <t>Perform equal-width binning with number of bins (numerical)</t>
+  </si>
+  <si>
+    <t>Perform equal-frequency binning with frequency (numerical)</t>
+  </si>
+  <si>
+    <t>Perform equal-frequency binning with number of bins (numerical)</t>
+  </si>
+  <si>
+    <t>Perform equal-width binning with width (categorical)</t>
+  </si>
+  <si>
+    <t>Perform equal-width binning with number of bins (categorical)</t>
+  </si>
+  <si>
+    <t>Perform equal-frequency binning with frequency (categorical)</t>
+  </si>
+  <si>
+    <t>Perform equal-frequency binning with number of bins (categorical)</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>(Calculate Statistical Table)</t>
+  </si>
+  <si>
+    <t>Compute stat table from df, column's bins settings, and good bad definition</t>
+  </si>
+  <si>
+    <t>Update auto bin panel when user changes the variable to be binned</t>
+  </si>
+  <si>
+    <t>Update the mixed chart when user changes the variable to be binned</t>
+  </si>
+  <si>
+    <t>Update statistic table (before) to none when user changes the variable to be binned</t>
+  </si>
+  <si>
+    <t>Update statistic table (after) when user changes the variable to be binned</t>
+  </si>
+  <si>
+    <t>Update the mixed chart when user clicked on the refresh button in auto bin panel</t>
+  </si>
+  <si>
+    <t>Update statistic table (after) when user clicked on the refresh button in auto bin panel</t>
+  </si>
+  <si>
+    <t>Update statistic table (before) when user clicked on the refresh button in auto bin panel</t>
+  </si>
+  <si>
+    <t>Save a temporary bin settings to storage when user clicked on the refresh button in auto bin panel</t>
+  </si>
+  <si>
+    <t>Remove the choice of equal-frequency binning if variable chosen to be binned is categorical</t>
+  </si>
+  <si>
+    <t>Update bin information when user clicked on a bar on the mixed chart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +457,14 @@
       <strike/>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -474,6 +530,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -805,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA56"/>
+  <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1290,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>8</v>
@@ -1313,7 +1376,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>8</v>
@@ -1425,7 +1488,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>8</v>
@@ -1471,7 +1534,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>8</v>
@@ -1494,7 +1557,7 @@
         <v>12</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1514,7 +1577,7 @@
         <v>12</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1534,7 +1597,7 @@
         <v>12</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1554,7 +1617,7 @@
         <v>12</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1574,7 +1637,7 @@
         <v>12</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1674,7 +1737,7 @@
         <v>12</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1685,7 +1748,7 @@
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
@@ -1725,7 +1788,7 @@
         <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>8</v>
@@ -1745,7 +1808,7 @@
         <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>8</v>
@@ -1765,7 +1828,7 @@
         <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>8</v>
@@ -1785,7 +1848,7 @@
         <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>8</v>
@@ -1801,31 +1864,121 @@
       <c r="A45" s="3">
         <v>44</v>
       </c>
+      <c r="B45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="5">
+        <v>45004</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
+      <c r="B46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="5">
+        <v>45015</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
+      <c r="B47" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="5">
+        <v>45015</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
+      <c r="B48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="5">
+        <v>45015</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
+      <c r="B49" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="5">
+        <v>45015</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
+      <c r="B50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="5">
+        <v>45015</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
@@ -1835,7 +1988,7 @@
         <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>8</v>
@@ -1844,29 +1997,47 @@
         <v>12</v>
       </c>
       <c r="F51" s="5">
-        <v>45004</v>
+        <v>45015</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C52" t="s">
-        <v>100</v>
+      <c r="C52" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C53" t="s">
-        <v>101</v>
+      <c r="C53" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -1874,10 +2045,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>118</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="5">
+        <v>45015</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -1885,10 +2065,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -1896,10 +2076,114 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update auto bin panel when var to bin changes
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A120448C-1079-40BD-8AAB-D3CEB22ADD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F6ED39-A516-4F0B-8251-8F1A8CE6E0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2070,6 +2070,15 @@
       <c r="C55" t="s">
         <v>127</v>
       </c>
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="5">
+        <v>45017</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
@@ -2080,6 +2089,15 @@
       </c>
       <c r="C56" t="s">
         <v>119</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="5">
+        <v>45017</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update mixed chart to real data & on change var to bin
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F6ED39-A516-4F0B-8251-8F1A8CE6E0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096EDC5C-4177-4843-9202-BE9B040BEE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>Update bin information when user clicked on a bar on the mixed chart</t>
+  </si>
+  <si>
+    <t>Update the mixed chart WOE line to real data</t>
+  </si>
+  <si>
+    <t>Update the mixed chart bars to real data</t>
   </si>
 </sst>
 </file>
@@ -870,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2110,6 +2116,15 @@
       <c r="C57" t="s">
         <v>122</v>
       </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="5">
+        <v>45017</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
@@ -2121,6 +2136,15 @@
       <c r="C58" t="s">
         <v>121</v>
       </c>
+      <c r="D58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="5">
+        <v>45017</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
@@ -2132,6 +2156,15 @@
       <c r="C59" t="s">
         <v>120</v>
       </c>
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="5">
+        <v>45017</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
@@ -2141,7 +2174,16 @@
         <v>32</v>
       </c>
       <c r="C60" t="s">
-        <v>124</v>
+        <v>130</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="5">
+        <v>45017</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2152,7 +2194,7 @@
         <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2163,7 +2205,7 @@
         <v>32</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2174,7 +2216,7 @@
         <v>32</v>
       </c>
       <c r="C63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2185,23 +2227,29 @@
         <v>32</v>
       </c>
       <c r="C64" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update woe to real data in mixed chart
</commit_message>
<xml_diff>
--- a/documentation/web-app-backlog.xlsx
+++ b/documentation/web-app-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinni\Desktop\Credit Scoring\credit-scoring-interactive-binning-web-app\credit-scoring-dataiku-pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096EDC5C-4177-4843-9202-BE9B040BEE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74CEB1-478A-47CC-8D07-68F62C446E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2195,6 +2195,15 @@
       </c>
       <c r="C61" t="s">
         <v>129</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="5">
+        <v>45017</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>